<commit_message>
extended test of collections, code repeats removed.
</commit_message>
<xml_diff>
--- a/Collection Benchmarks.xlsx
+++ b/Collection Benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\NetCracker\homeWork6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1090EFE-2AAE-439D-925D-C07436E5116A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB09FA0E-1252-4ABE-AD9E-3A1CFAB83CF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MyLinkedList" sheetId="5" r:id="rId1"/>
@@ -104,33 +104,6 @@
         <b/>
         <i/>
         <u/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Conclusion :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ArrayList always faster then LinkedList, need use ArrayList. Use LinkedList if yoo need isnert value in end or begin of list.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <u/>
         <sz val="16"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -192,6 +165,33 @@
   </si>
   <si>
     <t>MyLinkedList is faster. Faster due to fewer action checks</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Conclusion :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ArrayList nearly always faster then LinkedList, need use ArrayList. Use LinkedList if yoo need work with first or last value of list.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -537,12 +537,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -552,10 +546,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -14522,18 +14522,18 @@
       <c r="E2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
+      <c r="G2" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -14551,16 +14551,16 @@
       <c r="E3" s="12">
         <v>2467</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -14576,16 +14576,16 @@
       <c r="E4" s="13">
         <v>1464</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C5" s="23" t="s">
@@ -14597,16 +14597,16 @@
       <c r="E5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28"/>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
@@ -14624,16 +14624,16 @@
       <c r="E6" s="12">
         <v>1607552</v>
       </c>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
@@ -14649,16 +14649,16 @@
       <c r="E7" s="13">
         <v>1532310</v>
       </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
@@ -14676,16 +14676,16 @@
       <c r="E8" s="13">
         <v>1607552</v>
       </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
@@ -14701,16 +14701,16 @@
       <c r="E9" s="13">
         <v>1532310</v>
       </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -14728,16 +14728,16 @@
       <c r="E10" s="13">
         <v>1607552</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
@@ -14771,8 +14771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A21FCA-1FE5-49E6-B957-7F5436D568C1}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:Q10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14802,19 +14802,19 @@
       <c r="E2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
+      <c r="G2" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -14832,17 +14832,17 @@
       <c r="E3" s="12">
         <v>2467</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -14858,17 +14858,17 @@
       <c r="E4" s="13">
         <v>379</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C5" s="23">
@@ -14880,17 +14880,17 @@
       <c r="E5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="30"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
@@ -14908,17 +14908,17 @@
       <c r="E6" s="12">
         <v>1607552</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
@@ -14934,17 +14934,17 @@
       <c r="E7" s="13">
         <v>518324</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
@@ -14962,17 +14962,17 @@
       <c r="E8" s="13">
         <v>1607552</v>
       </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
@@ -14988,17 +14988,17 @@
       <c r="E9" s="13">
         <v>12</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -15016,17 +15016,17 @@
       <c r="E10" s="13">
         <v>1607552</v>
       </c>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
@@ -15061,7 +15061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE6A95E5-8F01-45E9-BEDC-A11E00F99956}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
@@ -15091,7 +15091,7 @@
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="30" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="5">
@@ -15108,7 +15108,7 @@
       <c r="A3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="27"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="11">
         <v>29</v>
       </c>
@@ -15123,7 +15123,7 @@
       <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="6">
         <v>51</v>
       </c>
@@ -15155,7 +15155,7 @@
       <c r="A6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="26"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="11">
         <v>15</v>
       </c>
@@ -15182,126 +15182,126 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
+      <c r="A25" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
+      <c r="A34" s="32"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
+      <c r="A35" s="32"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
+      <c r="A36" s="32"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -15345,25 +15345,25 @@
         <v>5</v>
       </c>
       <c r="G1" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
+        <v>24</v>
+      </c>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="30" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="5">
@@ -15375,24 +15375,24 @@
       <c r="E2" s="12">
         <v>2108</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="27"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="11">
         <v>11</v>
       </c>
@@ -15402,24 +15402,24 @@
       <c r="E3" s="13">
         <v>3162</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="6">
         <v>45</v>
       </c>
@@ -15429,18 +15429,18 @@
       <c r="E4" s="16">
         <v>9524</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
@@ -15458,24 +15458,24 @@
       <c r="E5" s="12">
         <v>1131</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="26"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="11">
         <v>5</v>
       </c>
@@ -15485,18 +15485,18 @@
       <c r="E6" s="13">
         <v>784</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
@@ -15512,18 +15512,18 @@
       <c r="E7" s="16">
         <v>8428</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="30"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
@@ -15541,24 +15541,24 @@
       <c r="E8" s="12">
         <v>1114</v>
       </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="30"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="26"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="11">
         <v>7</v>
       </c>
@@ -15568,18 +15568,18 @@
       <c r="E9" s="13">
         <v>1031</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
@@ -15595,18 +15595,18 @@
       <c r="E10" s="16">
         <v>13774</v>
       </c>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>